<commit_message>
removed duplicates from dataset, e.g. Target Group Analysis
</commit_message>
<xml_diff>
--- a/scraping/dataset/dataset.xlsx
+++ b/scraping/dataset/dataset.xlsx
@@ -5030,8 +5030,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5046,498 +5050,24 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>Sheet1!$B$437:$N$445</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="18"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Introduction to Database Design</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Introduction to Database Design</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Introduction to Database Design</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Introduction to Database Design</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Introduction to Database Design</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Introduction to Database Design</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>Introduction to Database Design</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>Introduction to Database Design</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>Introduction to Database Design</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>4,55</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>4,71</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>4,67</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>4,00</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>3,39</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>3,25</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>3,05</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>3,10</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>3,53</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="9">
-                    <c:v>3,37</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>4,94</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>4,43</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>5</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>5,11</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>3,88</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>4,86</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>5,6</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>5,05</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="9">
-                    <c:v>['Muhammad Ali Babar']</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>['Carsten Sch√ºrmann']</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>['Rasmus Ejlers M√∏gelberg']</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>['Rasmus Pagh']</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>['Rasmus Ejlers M√∏gelberg']</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>['Rasmus Pagh']</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>['Kennie Pontoppidan']</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>['Carsten Sch√ºrmann']</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>['Kennie Pontoppidan']</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="9">
-                    <c:v>2010a</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>2010b</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>2011a</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>2011b</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>2012a</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>2012b</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>2013a</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>2013b</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>2014a</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$O$437:$O$445</c:f>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>Sheet1!$B$437:$N$445</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="18"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Introduction to Database Design</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Introduction to Database Design</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Introduction to Database Design</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Introduction to Database Design</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Introduction to Database Design</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Introduction to Database Design</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>Introduction to Database Design</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>Introduction to Database Design</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>Introduction to Database Design</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>4,55</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>4,71</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>4,67</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>4,00</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>3,39</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>3,25</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>3,05</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>3,10</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>3,53</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="9">
-                    <c:v>3,37</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>4,94</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>4,43</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>5</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>5,11</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>3,88</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>4,86</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>5,6</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>5,05</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="9">
-                    <c:v>['Muhammad Ali Babar']</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>['Carsten Sch√ºrmann']</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>['Rasmus Ejlers M√∏gelberg']</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>['Rasmus Pagh']</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>['Rasmus Ejlers M√∏gelberg']</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>['Rasmus Pagh']</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>['Kennie Pontoppidan']</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>['Carsten Sch√ºrmann']</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>['Kennie Pontoppidan']</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="9">
-                    <c:v>2010a</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>2010b</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>2011a</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>2011b</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>2012a</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>2012b</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>2013a</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>2013b</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>2014a</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$P$437:$P$445</c:f>
-              <c:numCache>
-                <c:formatCode>@</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.94</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.57</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.62</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.62</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5.3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5.42</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="-2132118680"/>
-        <c:axId val="-2134723496"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="-2132118680"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2134723496"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="-2134723496"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="@" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132118680"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1371600</xdr:colOff>
-      <xdr:row>438</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
-      <xdr:row>452</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5869,7 +5399,7 @@
   <dimension ref="A1:P908"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5882,7 +5412,7 @@
     <col min="6" max="6" width="22.33203125" style="1" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="41.1640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="42.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" style="1" customWidth="1"/>
     <col min="10" max="10" width="17.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.33203125" style="2" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="13.5" style="2" hidden="1" customWidth="1"/>
@@ -51301,7 +50831,6 @@
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>